<commit_message>
Adjusted the HW5P2 results to be normalized
</commit_message>
<xml_diff>
--- a/HW5/HW5_Prob2/OMP_Results.xlsx
+++ b/HW5/HW5_Prob2/OMP_Results.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -160,33 +160,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$11</c:f>
+              <c:f>Sheet1!$C$4:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>181.78700000000001</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91.8</c:v>
+                  <c:v>0.50498660520279226</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61.119998899999999</c:v>
+                  <c:v>0.33621765527788011</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46.692999999999998</c:v>
+                  <c:v>0.25685555072694966</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49.417999999999999</c:v>
+                  <c:v>0.27184562152409136</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46.863999999999997</c:v>
+                  <c:v>0.25779621205036662</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>48.027000000000001</c:v>
+                  <c:v>0.26419380923828434</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>46.576000000000001</c:v>
+                  <c:v>0.25621194034776962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -201,11 +201,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="298900784"/>
-        <c:axId val="297883624"/>
+        <c:axId val="214133472"/>
+        <c:axId val="213932608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="298900784"/>
+        <c:axId val="214133472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -318,14 +318,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297883624"/>
+        <c:crossAx val="213932608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="297883624"/>
+        <c:axId val="213932608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -364,7 +365,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Execution Time (seconds)</a:t>
+                  <a:t>Execution Time (normalized)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -436,7 +437,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="298900784"/>
+        <c:crossAx val="214133472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1363,25 +1364,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1389,68 +1390,100 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
         <v>181.78700000000001</v>
       </c>
+      <c r="C4">
+        <f>B4/$B$4</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5">
         <v>91.8</v>
       </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C11" si="0">B5/$B$4</f>
+        <v>0.50498660520279226</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6">
         <v>61.119998899999999</v>
       </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.33621765527788011</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7">
         <v>46.692999999999998</v>
       </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.25685555072694966</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8">
         <v>49.417999999999999</v>
       </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.27184562152409136</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9">
         <v>46.863999999999997</v>
       </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.25779621205036662</v>
+      </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10">
         <v>48.027000000000001</v>
       </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.26419380923828434</v>
+      </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
       <c r="B11">
         <v>46.576000000000001</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0.25621194034776962</v>
       </c>
     </row>
   </sheetData>

</xml_diff>